<commit_message>
PISA 2015 scores by subject
</commit_message>
<xml_diff>
--- a/PisaScore2015.xlsx
+++ b/PisaScore2015.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasert/Dropbox/Excel_Instructor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C619B51-4932-A54B-A8AB-2CD3E094DFBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73AFEC2-F993-0D4F-99A5-FAC1F17E2D4A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="440" windowWidth="27720" windowHeight="17060" xr2:uid="{6482DD85-E40A-AC46-93C9-147A990C8273}"/>
+    <workbookView xWindow="700" yWindow="440" windowWidth="27720" windowHeight="17060" activeTab="2" xr2:uid="{6482DD85-E40A-AC46-93C9-147A990C8273}"/>
   </bookViews>
   <sheets>
     <sheet name="Math" sheetId="1" r:id="rId1"/>
     <sheet name="Science" sheetId="2" r:id="rId2"/>
     <sheet name="Reading" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,220 +38,220 @@
     <t>Reading</t>
   </si>
   <si>
-    <t> Singapore</t>
-  </si>
-  <si>
-    <t> Hong Kong</t>
-  </si>
-  <si>
-    <t> Macau</t>
-  </si>
-  <si>
-    <t> Taiwan</t>
-  </si>
-  <si>
-    <t> Japan</t>
-  </si>
-  <si>
-    <t> China</t>
-  </si>
-  <si>
-    <t> South Korea</t>
-  </si>
-  <si>
-    <t>  Switzerland</t>
-  </si>
-  <si>
-    <t> Estonia</t>
-  </si>
-  <si>
-    <t> Canada</t>
-  </si>
-  <si>
-    <t> Netherlands</t>
-  </si>
-  <si>
-    <t> Denmark</t>
-  </si>
-  <si>
-    <t> Finland</t>
-  </si>
-  <si>
-    <t> Slovenia</t>
-  </si>
-  <si>
-    <t> Belgium</t>
-  </si>
-  <si>
-    <t> Germany</t>
-  </si>
-  <si>
-    <t> Poland</t>
-  </si>
-  <si>
-    <t> Ireland</t>
-  </si>
-  <si>
-    <t> Norway</t>
-  </si>
-  <si>
-    <t> Austria</t>
-  </si>
-  <si>
-    <t> New Zealand</t>
-  </si>
-  <si>
-    <t> Vietnam</t>
-  </si>
-  <si>
-    <t> Russia</t>
-  </si>
-  <si>
-    <t> Sweden</t>
-  </si>
-  <si>
-    <t> Australia</t>
-  </si>
-  <si>
-    <t> France</t>
-  </si>
-  <si>
-    <t> United Kingdom</t>
-  </si>
-  <si>
-    <t> Czech Republic</t>
-  </si>
-  <si>
-    <t> Portugal</t>
-  </si>
-  <si>
-    <t> Italy</t>
-  </si>
-  <si>
-    <t> Iceland</t>
-  </si>
-  <si>
-    <t> Spain</t>
-  </si>
-  <si>
-    <t> Luxembourg</t>
-  </si>
-  <si>
-    <t> Latvia</t>
-  </si>
-  <si>
-    <t> Malta</t>
-  </si>
-  <si>
-    <t> Lithuania</t>
-  </si>
-  <si>
-    <t> Hungary</t>
-  </si>
-  <si>
-    <t> Slovakia</t>
-  </si>
-  <si>
-    <t> Israel</t>
-  </si>
-  <si>
-    <t> United States</t>
-  </si>
-  <si>
-    <t> Croatia</t>
-  </si>
-  <si>
-    <t> Kazakhstan</t>
-  </si>
-  <si>
-    <t> Greece</t>
-  </si>
-  <si>
-    <t> Romania</t>
-  </si>
-  <si>
-    <t> Bulgaria</t>
-  </si>
-  <si>
-    <t> Cyprus</t>
-  </si>
-  <si>
-    <t> United Arab Emirates</t>
-  </si>
-  <si>
-    <t> Chile</t>
-  </si>
-  <si>
-    <t> Turkey</t>
-  </si>
-  <si>
-    <t> Moldova</t>
-  </si>
-  <si>
-    <t> Uruguay</t>
-  </si>
-  <si>
-    <t> Montenegro</t>
-  </si>
-  <si>
-    <t> Trinidad and Tobago</t>
-  </si>
-  <si>
-    <t> Thailand</t>
-  </si>
-  <si>
-    <t> Albania</t>
-  </si>
-  <si>
-    <t> Mexico</t>
-  </si>
-  <si>
-    <t> Georgia</t>
-  </si>
-  <si>
-    <t> Qatar</t>
-  </si>
-  <si>
-    <t> Costa Rica</t>
-  </si>
-  <si>
-    <t> Lebanon</t>
-  </si>
-  <si>
-    <t> Colombia</t>
-  </si>
-  <si>
-    <t> Peru</t>
-  </si>
-  <si>
-    <t> Indonesia</t>
-  </si>
-  <si>
-    <t> Jordan</t>
-  </si>
-  <si>
-    <t> Brazil</t>
-  </si>
-  <si>
-    <t> Macedonia</t>
-  </si>
-  <si>
-    <t> Tunisia</t>
-  </si>
-  <si>
-    <t> Kosovo</t>
-  </si>
-  <si>
-    <t> Algeria</t>
-  </si>
-  <si>
-    <t> Dominican Republic</t>
-  </si>
-  <si>
     <t>Rank</t>
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>HongKong</t>
+  </si>
+  <si>
+    <t>Macau</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>SouthKorea</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>NewZealand</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>UnitedKingdom</t>
+  </si>
+  <si>
+    <t>CzechRepublic</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>UnitedStates</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>UnitedArabEmirates</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>TrinidadandTobago</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>CostaRica</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>DominicanRepublic</t>
   </si>
 </sst>
 </file>
@@ -605,18 +605,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AD4BBB-8BE9-4247-972A-9F1325213B8E}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -627,7 +625,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>564</v>
@@ -638,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>548</v>
@@ -649,7 +647,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>544</v>
@@ -660,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>542</v>
@@ -671,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>532</v>
@@ -682,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>531</v>
@@ -693,7 +691,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>524</v>
@@ -704,7 +702,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>521</v>
@@ -715,7 +713,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>520</v>
@@ -726,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>516</v>
@@ -737,7 +735,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>512</v>
@@ -748,7 +746,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>511</v>
@@ -759,7 +757,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>511</v>
@@ -770,7 +768,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>510</v>
@@ -781,7 +779,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>507</v>
@@ -792,7 +790,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>506</v>
@@ -803,7 +801,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>504</v>
@@ -814,7 +812,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>504</v>
@@ -825,7 +823,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>502</v>
@@ -836,7 +834,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>497</v>
@@ -847,7 +845,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>495</v>
@@ -858,7 +856,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>495</v>
@@ -869,7 +867,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>494</v>
@@ -880,7 +878,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25">
         <v>494</v>
@@ -891,7 +889,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>494</v>
@@ -902,7 +900,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>493</v>
@@ -913,7 +911,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>492</v>
@@ -924,7 +922,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>492</v>
@@ -935,7 +933,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C30">
         <v>492</v>
@@ -946,7 +944,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>490</v>
@@ -957,7 +955,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C32">
         <v>488</v>
@@ -968,7 +966,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C33">
         <v>486</v>
@@ -979,7 +977,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>486</v>
@@ -990,7 +988,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C35">
         <v>482</v>
@@ -1001,7 +999,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C36">
         <v>479</v>
@@ -1012,7 +1010,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>478</v>
@@ -1023,7 +1021,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C38">
         <v>477</v>
@@ -1034,7 +1032,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C39">
         <v>475</v>
@@ -1045,7 +1043,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C40">
         <v>470</v>
@@ -1056,7 +1054,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C41">
         <v>470</v>
@@ -1067,7 +1065,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C42">
         <v>464</v>
@@ -1078,7 +1076,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43">
         <v>460</v>
@@ -1089,7 +1087,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C44">
         <v>454</v>
@@ -1100,7 +1098,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C45">
         <v>444</v>
@@ -1111,7 +1109,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C46">
         <v>441</v>
@@ -1122,7 +1120,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47">
         <v>437</v>
@@ -1133,7 +1131,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C48">
         <v>427</v>
@@ -1144,7 +1142,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C49">
         <v>423</v>
@@ -1155,7 +1153,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C50">
         <v>420</v>
@@ -1166,7 +1164,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C51">
         <v>420</v>
@@ -1177,7 +1175,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C52">
         <v>418</v>
@@ -1188,7 +1186,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C53">
         <v>418</v>
@@ -1199,7 +1197,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54">
         <v>417</v>
@@ -1210,7 +1208,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C55">
         <v>415</v>
@@ -1221,7 +1219,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C56">
         <v>413</v>
@@ -1232,7 +1230,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C57">
         <v>408</v>
@@ -1243,7 +1241,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58">
         <v>404</v>
@@ -1254,7 +1252,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59">
         <v>402</v>
@@ -1265,7 +1263,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60">
         <v>400</v>
@@ -1276,7 +1274,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61">
         <v>396</v>
@@ -1287,7 +1285,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C62">
         <v>390</v>
@@ -1298,7 +1296,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C63">
         <v>387</v>
@@ -1309,7 +1307,7 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C64">
         <v>386</v>
@@ -1320,7 +1318,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C65">
         <v>380</v>
@@ -1331,7 +1329,7 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C66">
         <v>377</v>
@@ -1342,7 +1340,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C67">
         <v>371</v>
@@ -1353,7 +1351,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C68">
         <v>367</v>
@@ -1364,7 +1362,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C69">
         <v>362</v>
@@ -1375,7 +1373,7 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C70">
         <v>360</v>
@@ -1386,7 +1384,7 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C71">
         <v>328</v>
@@ -1410,10 +1408,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1424,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>556</v>
@@ -1435,7 +1433,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>538</v>
@@ -1446,7 +1444,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>534</v>
@@ -1457,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>532</v>
@@ -1468,7 +1466,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>531</v>
@@ -1479,7 +1477,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>529</v>
@@ -1490,7 +1488,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>528</v>
@@ -1501,7 +1499,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>525</v>
@@ -1512,7 +1510,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>523</v>
@@ -1523,7 +1521,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>518</v>
@@ -1534,7 +1532,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>516</v>
@@ -1545,7 +1543,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13">
         <v>513</v>
@@ -1556,7 +1554,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>513</v>
@@ -1567,7 +1565,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>510</v>
@@ -1578,7 +1576,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>509</v>
@@ -1589,7 +1587,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>509</v>
@@ -1600,7 +1598,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>509</v>
@@ -1611,7 +1609,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>506</v>
@@ -1622,7 +1620,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>503</v>
@@ -1633,7 +1631,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>502</v>
@@ -1644,7 +1642,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>502</v>
@@ -1655,7 +1653,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>501</v>
@@ -1666,7 +1664,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>501</v>
@@ -1677,7 +1675,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25">
         <v>498</v>
@@ -1688,7 +1686,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C26">
         <v>496</v>
@@ -1699,7 +1697,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>495</v>
@@ -1710,7 +1708,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>495</v>
@@ -1721,7 +1719,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29">
         <v>493</v>
@@ -1732,7 +1730,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>493</v>
@@ -1743,7 +1741,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>493</v>
@@ -1754,7 +1752,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <v>490</v>
@@ -1765,7 +1763,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C33">
         <v>487</v>
@@ -1776,7 +1774,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>483</v>
@@ -1787,7 +1785,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>481</v>
@@ -1798,7 +1796,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>477</v>
@@ -1809,7 +1807,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>475</v>
@@ -1820,7 +1818,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>475</v>
@@ -1831,7 +1829,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C39">
         <v>473</v>
@@ -1842,7 +1840,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C40">
         <v>467</v>
@@ -1853,7 +1851,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C41">
         <v>465</v>
@@ -1864,7 +1862,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>461</v>
@@ -1875,7 +1873,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43">
         <v>456</v>
@@ -1886,7 +1884,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C44">
         <v>455</v>
@@ -1897,7 +1895,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C45">
         <v>447</v>
@@ -1908,7 +1906,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C46">
         <v>446</v>
@@ -1919,7 +1917,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C47">
         <v>437</v>
@@ -1930,7 +1928,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>435</v>
@@ -1941,7 +1939,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C49">
         <v>435</v>
@@ -1952,7 +1950,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C50">
         <v>433</v>
@@ -1963,7 +1961,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C51">
         <v>428</v>
@@ -1974,7 +1972,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C52">
         <v>427</v>
@@ -1985,7 +1983,7 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C53">
         <v>425</v>
@@ -1996,7 +1994,7 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54">
         <v>425</v>
@@ -2007,7 +2005,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C55">
         <v>421</v>
@@ -2018,7 +2016,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C56">
         <v>420</v>
@@ -2029,7 +2027,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C57">
         <v>418</v>
@@ -2040,7 +2038,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C58">
         <v>416</v>
@@ -2051,7 +2049,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C59">
         <v>404</v>
@@ -2062,7 +2060,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C60">
         <v>411</v>
@@ -2073,7 +2071,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C61">
         <v>411</v>
@@ -2084,7 +2082,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C62">
         <v>409</v>
@@ -2095,7 +2093,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C63">
         <v>403</v>
@@ -2106,7 +2104,7 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>401</v>
@@ -2117,7 +2115,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C65">
         <v>397</v>
@@ -2128,7 +2126,7 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C66">
         <v>386</v>
@@ -2139,7 +2137,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C67">
         <v>386</v>
@@ -2150,7 +2148,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C68">
         <v>384</v>
@@ -2161,7 +2159,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C69">
         <v>378</v>
@@ -2172,7 +2170,7 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C70">
         <v>376</v>
@@ -2183,7 +2181,7 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C71">
         <v>332</v>
@@ -2198,18 +2196,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D756435-9F58-0841-A8F2-9DCC7D6AF44D}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2220,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>535</v>
@@ -2231,7 +2229,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>527</v>
@@ -2242,7 +2240,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>527</v>
@@ -2253,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>526</v>
@@ -2264,7 +2262,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>521</v>
@@ -2275,7 +2273,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>519</v>
@@ -2286,7 +2284,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>517</v>
@@ -2297,7 +2295,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>516</v>
@@ -2308,7 +2306,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>513</v>
@@ -2319,7 +2317,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>509</v>
@@ -2330,7 +2328,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>509</v>
@@ -2341,7 +2339,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>509</v>
@@ -2352,7 +2350,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>506</v>
@@ -2363,7 +2361,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>505</v>
@@ -2374,7 +2372,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>503</v>
@@ -2385,7 +2383,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>503</v>
@@ -2396,7 +2394,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>500</v>
@@ -2407,7 +2405,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>500</v>
@@ -2418,7 +2416,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>499</v>
@@ -2429,7 +2427,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>499</v>
@@ -2440,7 +2438,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>498</v>
@@ -2451,7 +2449,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>498</v>
@@ -2462,7 +2460,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24">
         <v>497</v>
@@ -2473,7 +2471,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25">
         <v>497</v>
@@ -2484,7 +2482,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <v>496</v>
@@ -2495,7 +2493,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>495</v>
@@ -2506,7 +2504,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>494</v>
@@ -2517,7 +2515,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>492</v>
@@ -2528,7 +2526,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C30">
         <v>488</v>
@@ -2539,7 +2537,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>487</v>
@@ -2550,7 +2548,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C32">
         <v>487</v>
@@ -2561,7 +2559,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C33">
         <v>487</v>
@@ -2572,7 +2570,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C34">
         <v>485</v>
@@ -2583,7 +2581,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>485</v>
@@ -2594,7 +2592,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>482</v>
@@ -2605,7 +2603,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>481</v>
@@ -2616,7 +2614,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>479</v>
@@ -2627,7 +2625,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>472</v>
@@ -2638,7 +2636,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>470</v>
@@ -2649,7 +2647,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C41">
         <v>467</v>
@@ -2660,7 +2658,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C42">
         <v>459</v>
@@ -2671,7 +2669,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C43">
         <v>453</v>
@@ -2682,7 +2680,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C44">
         <v>447</v>
@@ -2693,7 +2691,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>443</v>
@@ -2704,7 +2702,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>437</v>
@@ -2715,7 +2713,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C47">
         <v>434</v>
@@ -2726,7 +2724,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C48">
         <v>434</v>
@@ -2737,7 +2735,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C49">
         <v>432</v>
@@ -2748,7 +2746,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C50">
         <v>428</v>
@@ -2759,7 +2757,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C51">
         <v>427</v>
@@ -2770,7 +2768,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C52">
         <v>427</v>
@@ -2781,7 +2779,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C53">
         <v>427</v>
@@ -2792,7 +2790,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C54">
         <v>427</v>
@@ -2803,7 +2801,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C55">
         <v>425</v>
@@ -2814,7 +2812,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C56">
         <v>423</v>
@@ -2825,7 +2823,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C57">
         <v>416</v>
@@ -2836,7 +2834,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C58">
         <v>409</v>
@@ -2847,7 +2845,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C59">
         <v>408</v>
@@ -2858,7 +2856,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C60">
         <v>407</v>
@@ -2869,7 +2867,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C61">
         <v>405</v>
@@ -2880,7 +2878,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C62">
         <v>402</v>
@@ -2891,7 +2889,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C63">
         <v>401</v>
@@ -2902,7 +2900,7 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C64">
         <v>398</v>
@@ -2913,7 +2911,7 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C65">
         <v>397</v>
@@ -2924,7 +2922,7 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C66">
         <v>361</v>
@@ -2935,7 +2933,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C67">
         <v>358</v>
@@ -2946,7 +2944,7 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C68">
         <v>352</v>
@@ -2957,7 +2955,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C69">
         <v>350</v>
@@ -2968,7 +2966,7 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C70">
         <v>347</v>
@@ -2979,7 +2977,7 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C71">
         <v>347</v>

</xml_diff>